<commit_message>
Updated log and finished ExU
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G54-0624-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G54-0624-350-1201.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rico\Desktop\ENSC 350 Final Project\ENSC350FP\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9229A720-FA14-4238-9242-23BE35A3831E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B76FBCC-C9FE-4753-A5F8-1CAD961B2224}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6075" yWindow="3840" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="5865" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log - Part 1" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t>Worked on SLL, SRL, and SRA</t>
+  </si>
+  <si>
+    <t>Worked on Shift Unit</t>
+  </si>
+  <si>
+    <t>Finished Shift Unit, combined with Execution Unit and Functional simulation worked</t>
   </si>
 </sst>
 </file>
@@ -2892,7 +2898,7 @@
   <dimension ref="A1:I782"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3025,28 +3031,46 @@
     </row>
     <row r="8" spans="1:9" ht="24.95" customHeight="1">
       <c r="A8" s="33"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="23"/>
+      <c r="B8" s="14">
+        <v>624</v>
+      </c>
+      <c r="C8" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D8" s="20">
+        <v>0.76527777777777783</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="F8" s="34"/>
-      <c r="G8" s="17"/>
+      <c r="G8" s="17" t="s">
+        <v>32</v>
+      </c>
       <c r="H8" s="27">
         <f t="shared" ref="H8:H71" si="1">(E8-D8)*24</f>
-        <v>0</v>
+        <v>3.6333333333333311</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="24.95" customHeight="1">
       <c r="A9" s="33"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="23"/>
+      <c r="C9" s="22">
+        <v>43931</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0.99652777777777779</v>
+      </c>
       <c r="F9" s="34"/>
-      <c r="G9" s="17"/>
+      <c r="G9" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="H9" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5833333333333357</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="24.95" customHeight="1">
@@ -3950,7 +3974,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>3.1833333333333327</v>
+        <v>8.3999999999999986</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1"/>

</xml_diff>

<commit_message>
Created submission folder for documentation and moved some documentation over
</commit_message>
<xml_diff>
--- a/ExU/Documentation/FP-log-G54-0624-350-1201.xlsx
+++ b/ExU/Documentation/FP-log-G54-0624-350-1201.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rico\Desktop\ENSC 350 Final Project\ENSC350FP\ExU\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F147D729-AB08-412A-97EB-5C3DFC2046DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D28C51E-C5D5-4C6B-B18F-F0A95C16885F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3885" yWindow="3630" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="1725" yWindow="1800" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log - Part 1" sheetId="5" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -209,6 +209,21 @@
   </si>
   <si>
     <t>Done with Documenting Design Entities for the Barrel Shifters and fixed format for the wave screeenshots</t>
+  </si>
+  <si>
+    <t>Deon with Documenting Design Entities for all our designs</t>
+  </si>
+  <si>
+    <t>Adding Comments to Source code</t>
+  </si>
+  <si>
+    <t>Worked on improving report</t>
+  </si>
+  <si>
+    <t>Done with discussion on the observation and results of our functional simulation</t>
+  </si>
+  <si>
+    <t>Did a quick proofread and setup the folder for our documentation</t>
   </si>
 </sst>
 </file>
@@ -2924,8 +2939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD091BD6-3364-44DE-8BB4-985458F62AD8}">
   <dimension ref="A1:I782"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3311,67 +3326,117 @@
     </row>
     <row r="19" spans="1:8" ht="24.95" customHeight="1">
       <c r="A19" s="33"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="23"/>
+      <c r="B19" s="14">
+        <v>624</v>
+      </c>
+      <c r="C19" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D19" s="20">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E19" s="23">
+        <v>0.73611111111111116</v>
+      </c>
       <c r="F19" s="34"/>
-      <c r="G19" s="17"/>
+      <c r="G19" s="17" t="s">
+        <v>43</v>
+      </c>
       <c r="H19" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.6666666666666687</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="24.95" customHeight="1">
       <c r="A20" s="33"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="23"/>
+      <c r="B20" s="14">
+        <v>624</v>
+      </c>
+      <c r="C20" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D20" s="20">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="E20" s="23">
+        <v>0.78333333333333333</v>
+      </c>
       <c r="F20" s="34"/>
-      <c r="G20" s="17"/>
+      <c r="G20" s="17" t="s">
+        <v>44</v>
+      </c>
       <c r="H20" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.133333333333332</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="24.95" customHeight="1">
       <c r="A21" s="33"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="23"/>
+      <c r="B21" s="14">
+        <v>624</v>
+      </c>
+      <c r="C21" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D21" s="20">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E21" s="23">
+        <v>0.89930555555555547</v>
+      </c>
       <c r="F21" s="34"/>
-      <c r="G21" s="17"/>
+      <c r="G21" s="17" t="s">
+        <v>45</v>
+      </c>
       <c r="H21" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5833333333333304</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="24.95" customHeight="1">
       <c r="A22" s="33"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="23"/>
+      <c r="B22" s="14">
+        <v>624</v>
+      </c>
+      <c r="C22" s="22">
+        <v>43937</v>
+      </c>
+      <c r="D22" s="20">
+        <v>0.89930555555555547</v>
+      </c>
+      <c r="E22" s="23">
+        <v>0.95138888888888884</v>
+      </c>
       <c r="F22" s="34"/>
-      <c r="G22" s="17"/>
+      <c r="G22" s="17" t="s">
+        <v>46</v>
+      </c>
       <c r="H22" s="27">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.2500000000000009</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="24.95" customHeight="1">
       <c r="A23" s="33"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="23"/>
+      <c r="B23" s="14">
+        <v>624</v>
+      </c>
+      <c r="C23" s="22">
+        <v>43938</v>
+      </c>
+      <c r="D23" s="20">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="E23" s="23">
+        <v>0.70277777777777783</v>
+      </c>
       <c r="F23" s="34"/>
-      <c r="G23" s="17"/>
+      <c r="G23" s="17" t="s">
+        <v>47</v>
+      </c>
       <c r="H23" s="27">
         <f>(E23-D23)*24</f>
-        <v>0</v>
+        <v>0.61666666666666714</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="24.95" customHeight="1">
@@ -4093,7 +4158,7 @@
       <c r="F79" s="30"/>
       <c r="H79" s="29">
         <f>SUM(H6:H78)</f>
-        <v>17.233333333333331</v>
+        <v>23.483333333333327</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="24.95" customHeight="1"/>

</xml_diff>